<commit_message>
Doxygen + Tests formatiert
</commit_message>
<xml_diff>
--- a/diagramme/BossTests.xlsx
+++ b/diagramme/BossTests.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Youssef\AppData\Local\Temp\MicrosoftEdgeDownloads\219c8e24-69fc-4062-82b8-52bd6d19de1b\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Youssef\Desktop\UNI\S4\ComputerspielEntwicklung\DasSpiel\anfaengerpraktikum\diagramme\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41CDE81D-25E3-4D9C-9070-03AE9D1FCC42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6579818A-FEBB-4287-A2ED-CA01650F38E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="59">
   <si>
     <t>Anforderung</t>
   </si>
@@ -73,12 +73,6 @@
     <t>Der Boss belebt alle gestorbenen Gegner im Raum wieder, sobald er unter 50 % Lebenspunkte fällt.</t>
   </si>
   <si>
-    <t>Wenn der Spieler in den Detectionbereich eines Bosss läuft, muss der Boss den Spieler anfangen zu verfolgen</t>
-  </si>
-  <si>
-    <t>Wenn der Spieler den Pursuingbereich eines Bosss verlässt, muss der Boss den Spieler aufhören zu verfolgen</t>
-  </si>
-  <si>
     <t>Wenn eine Szene geladen wird, hat der Boss eine fixe deterministische Startposition.</t>
   </si>
   <si>
@@ -97,9 +91,6 @@
     <t>Wenn ein Boss Stirbt, muss der Spieler die beim Boss festgelegte Anzahl an Sünden bekommen.</t>
   </si>
   <si>
-    <t>Wenn ein Boss vor einer Wand oder auf dem Boden stehte muss er mit diesen Objekten kollidieren.</t>
-  </si>
-  <si>
     <t>Wenn ein Spieler vor dem Boss steht, darf der Boss nicht durch den Spieler laufen.</t>
   </si>
   <si>
@@ -194,13 +185,25 @@
   </si>
   <si>
     <t>2.2.3.6.3</t>
+  </si>
+  <si>
+    <t>Wenn der Boss vor einer Wand oder auf dem Boden stehte muss er mit diesen Objekten kollidieren.</t>
+  </si>
+  <si>
+    <t>Wenn der Spieler in den Detectionbereich des Bosses läuft, muss der Boss den Spieler anfangen zu verfolgen</t>
+  </si>
+  <si>
+    <t>Wenn der Spieler den Pursuingbereich eines Bosses verlässt, muss der Boss den Spieler aufhören zu verfolgen</t>
+  </si>
+  <si>
+    <t>Tests für Boss</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -211,6 +214,14 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -264,14 +275,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -576,260 +599,277 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E14"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="86.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="97" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="74.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.88671875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="21.5546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="24.109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="8.5546875" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.4">
+      <c r="A1" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+    <row r="3" spans="1:5" ht="72" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="73.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="87.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="B6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+      <c r="E6" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="61.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="2" t="s">
+      <c r="B7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
+      <c r="E7" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="67.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="2" t="s">
+      <c r="B8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+      <c r="E8" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="85.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="2" t="s">
+      <c r="B9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
+      <c r="E9" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="2" t="s">
+      <c r="B10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
+      <c r="E10" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="2" t="s">
+      <c r="B11" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
+      <c r="E11" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="60.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="2" t="s">
+      <c r="B12" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D12" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
+      <c r="E12" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="2" t="s">
+      <c r="C13" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D13" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="2" t="s">
+      <c r="E13" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="64.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D14" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E10" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="2" t="s">
+      <c r="E14" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D15" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E11" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>43</v>
+      <c r="E15" s="5" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="95" fitToHeight="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>